<commit_message>
deleted the old excel file. Changed the word name to username
</commit_message>
<xml_diff>
--- a/requirements (version 1).xlsb.xlsx
+++ b/requirements (version 1).xlsb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomas\Desktop\3 vikna\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7C31B2-DBB9-4A71-B370-098834143E83}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EB6082-FAA2-4E62-9A0E-858CF2D87B87}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{292ADBA8-52A5-47D6-97C7-E12D992943EB}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -52,18 +51,12 @@
     <t>A</t>
   </si>
   <si>
-    <t>Should be possible to create a profile consisting of a name</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
     <t>Should be possible to add an image to ones own profile</t>
   </si>
   <si>
-    <t>Should be possible to edit name in ones own profile</t>
-  </si>
-  <si>
     <t>Should be possible to change image in ones own profile</t>
   </si>
   <si>
@@ -185,6 +178,12 @@
   </si>
   <si>
     <t>Róslín</t>
+  </si>
+  <si>
+    <t>Should be possible to create a profile consisting of a username</t>
+  </si>
+  <si>
+    <t>Should be possible to edit/add name in ones own profile other than username</t>
   </si>
 </sst>
 </file>
@@ -605,14 +604,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A29ECF-1B85-49A7-9822-BF06B096B68E}">
   <dimension ref="B3:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="67.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="11" max="11" width="60.85546875" bestFit="1" customWidth="1"/>
@@ -645,10 +644,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>5</v>
@@ -659,16 +658,16 @@
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -676,10 +675,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>5</v>
@@ -690,10 +689,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>5</v>
@@ -704,10 +703,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>5</v>
@@ -718,10 +717,10 @@
         <v>6</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>5</v>
@@ -732,16 +731,16 @@
         <v>7</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -749,10 +748,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>5</v>
@@ -763,10 +762,10 @@
         <v>9</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>5</v>
@@ -777,16 +776,16 @@
         <v>10</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>5</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -794,10 +793,10 @@
         <v>11</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>5</v>
@@ -808,10 +807,10 @@
         <v>12</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>5</v>
@@ -822,10 +821,10 @@
         <v>13</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>5</v>
@@ -836,10 +835,10 @@
         <v>14</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>5</v>
@@ -850,16 +849,16 @@
         <v>15</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -867,13 +866,13 @@
         <v>16</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -881,13 +880,13 @@
         <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -895,13 +894,13 @@
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
@@ -909,13 +908,13 @@
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
@@ -923,13 +922,13 @@
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -937,13 +936,13 @@
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -951,13 +950,13 @@
         <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
@@ -965,13 +964,13 @@
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
@@ -979,13 +978,13 @@
         <v>24</v>
       </c>
       <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" t="s">
         <v>39</v>
       </c>
-      <c r="D28" t="s">
-        <v>41</v>
-      </c>
       <c r="E28" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
@@ -993,18 +992,18 @@
         <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1015,10 +1014,10 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>5</v>
@@ -1029,10 +1028,10 @@
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>5</v>
@@ -1043,10 +1042,10 @@
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>5</v>
@@ -1057,10 +1056,10 @@
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>5</v>
@@ -1071,10 +1070,10 @@
         <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D35" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>5</v>
@@ -1085,10 +1084,10 @@
         <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D36" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>5</v>
@@ -1099,10 +1098,10 @@
         <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>5</v>
@@ -1113,10 +1112,10 @@
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D38" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>5</v>
@@ -1127,10 +1126,10 @@
         <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D39" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>5</v>
@@ -1141,10 +1140,10 @@
         <v>10</v>
       </c>
       <c r="C40" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D40" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
fixed a grammar error in excel
</commit_message>
<xml_diff>
--- a/requirements (version 1).xlsb.xlsx
+++ b/requirements (version 1).xlsb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomas\Desktop\3 vikna\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EB6082-FAA2-4E62-9A0E-858CF2D87B87}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705400D9-E939-4247-B364-08C9A1CBAAA8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{292ADBA8-52A5-47D6-97C7-E12D992943EB}"/>
+    <workbookView xWindow="-8790" yWindow="1800" windowWidth="18000" windowHeight="9360" xr2:uid="{292ADBA8-52A5-47D6-97C7-E12D992943EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
     <t>Should be possible to create a profile consisting of a username</t>
   </si>
   <si>
-    <t>Should be possible to edit/add name in ones own profile other than username</t>
+    <t>Should be possible to edit name in ones own profile</t>
   </si>
 </sst>
 </file>
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A29ECF-1B85-49A7-9822-BF06B096B68E}">
   <dimension ref="B3:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Deleted the highlighting over my part in the excel since it was done
</commit_message>
<xml_diff>
--- a/requirements (version 1).xlsb.xlsx
+++ b/requirements (version 1).xlsb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomas\Desktop\3 vikna\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705400D9-E939-4247-B364-08C9A1CBAAA8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04868AEA-888E-44E6-A206-725D7C9F671B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8790" yWindow="1800" windowWidth="18000" windowHeight="9360" xr2:uid="{292ADBA8-52A5-47D6-97C7-E12D992943EB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{292ADBA8-52A5-47D6-97C7-E12D992943EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -206,7 +206,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,12 +240,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -284,8 +278,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -605,7 +599,7 @@
   <dimension ref="B3:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,6 +823,7 @@
       <c r="E17" s="12" t="s">
         <v>5</v>
       </c>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
@@ -843,6 +838,7 @@
       <c r="E18" s="12" t="s">
         <v>5</v>
       </c>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="11">
@@ -874,6 +870,7 @@
       <c r="E20" s="12" t="s">
         <v>6</v>
       </c>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21">

</xml_diff>

<commit_message>
added a requirement function, edited requirement list
</commit_message>
<xml_diff>
--- a/requirements (version 1).xlsb.xlsx
+++ b/requirements (version 1).xlsb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomas\Desktop\3 vikna\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbval\Desktop\3Vikna\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04868AEA-888E-44E6-A206-725D7C9F671B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616D043E-1D8A-4BAC-B63A-E6D6B9665C36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{292ADBA8-52A5-47D6-97C7-E12D992943EB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{292ADBA8-52A5-47D6-97C7-E12D992943EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="48">
   <si>
     <t>Number</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Should be possible to filter by type of product on catalogue site</t>
   </si>
   <si>
-    <t>Should be possible to search by name on catalogue site</t>
-  </si>
-  <si>
     <t>Should be possible to order by price of prodcuts on catalogue site</t>
   </si>
   <si>
@@ -168,22 +165,16 @@
     <t>More than 90% of users should be able to navigate the website</t>
   </si>
   <si>
-    <t>BERGLIND</t>
-  </si>
-  <si>
-    <t>Hörður</t>
-  </si>
-  <si>
-    <t>Jevgenija</t>
-  </si>
-  <si>
-    <t>Róslín</t>
-  </si>
-  <si>
     <t>Should be possible to create a profile consisting of a username</t>
   </si>
   <si>
     <t>Should be possible to edit name in ones own profile</t>
+  </si>
+  <si>
+    <t>Should be possible to search by name of a product from anywhere on the site</t>
+  </si>
+  <si>
+    <t>Should be possible to remove a product from the cart</t>
   </si>
 </sst>
 </file>
@@ -206,7 +197,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,24 +216,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -256,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -264,18 +237,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -596,22 +557,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A29ECF-1B85-49A7-9822-BF06B096B68E}">
-  <dimension ref="B3:F40"/>
+  <dimension ref="B3:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="72.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="60.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.265625" customWidth="1"/>
+    <col min="5" max="5" width="12.73046875" customWidth="1"/>
+    <col min="11" max="11" width="60.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -625,7 +586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -633,21 +594,21 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B5" s="5">
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B6" s="5">
         <v>2</v>
       </c>
@@ -655,16 +616,13 @@
         <v>10</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B7" s="5">
         <v>3</v>
       </c>
@@ -672,13 +630,13 @@
         <v>9</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B8" s="5">
         <v>4</v>
       </c>
@@ -686,388 +644,377 @@
         <v>11</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B9" s="5">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B10" s="5">
+        <v>6</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B11" s="5">
+        <v>7</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B12" s="5">
+        <v>8</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B13" s="5">
+        <v>9</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B14" s="5">
+        <v>10</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B15" s="5">
+        <v>11</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B16" s="5">
+        <v>12</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B17" s="5">
+        <v>13</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B18" s="5">
+        <v>14</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="7">
-        <v>5</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="7">
+      <c r="E18" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B19" s="5">
+        <v>15</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B20" s="5">
+        <v>16</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="7">
-        <v>7</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B21" s="5">
+        <v>17</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="7">
-        <v>8</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="9">
-        <v>9</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="9">
-        <v>10</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="9">
-        <v>11</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="9">
-        <v>12</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="11">
-        <v>13</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="11">
-        <v>14</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="11">
-        <v>15</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="12" t="s">
+      <c r="D21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="11">
-        <v>16</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="11"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <v>17</v>
-      </c>
-      <c r="C21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B22">
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B23">
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B24">
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B25">
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B26">
         <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B27">
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B28">
         <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B29">
         <v>25</v>
       </c>
       <c r="C29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B30">
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D29" t="s">
-        <v>36</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="D32" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
         <v>29</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D34" t="s">
         <v>35</v>
       </c>
-      <c r="E31" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32">
-        <v>2</v>
-      </c>
-      <c r="C32" t="s">
-        <v>44</v>
-      </c>
-      <c r="D32" t="s">
-        <v>35</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33">
-        <v>3</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="E34" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35" t="s">
         <v>30</v>
-      </c>
-      <c r="D33" t="s">
-        <v>36</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34">
-        <v>4</v>
-      </c>
-      <c r="C34" t="s">
-        <v>31</v>
-      </c>
-      <c r="D34" t="s">
-        <v>36</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35">
-        <v>5</v>
-      </c>
-      <c r="C35" t="s">
-        <v>43</v>
       </c>
       <c r="D35" t="s">
         <v>35</v>
@@ -1076,40 +1023,40 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B37">
         <v>6</v>
-      </c>
-      <c r="C36" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" t="s">
-        <v>36</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37">
-        <v>7</v>
       </c>
       <c r="C37" t="s">
         <v>32</v>
       </c>
       <c r="D37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B38">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D38" t="s">
         <v>35</v>
@@ -1118,31 +1065,45 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="3">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B39">
+        <v>8</v>
+      </c>
+      <c r="C39" t="s">
+        <v>33</v>
+      </c>
+      <c r="D39" t="s">
+        <v>34</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B40" s="3">
         <v>9</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B41">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
         <v>40</v>
       </c>
-      <c r="D39" t="s">
-        <v>35</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40">
-        <v>10</v>
-      </c>
-      <c r="C40" t="s">
-        <v>41</v>
-      </c>
-      <c r="D40" t="s">
-        <v>35</v>
-      </c>
-      <c r="E40" s="4" t="s">
+      <c r="D41" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" s="4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated the requirement list
</commit_message>
<xml_diff>
--- a/requirements (version 1).xlsb.xlsx
+++ b/requirements (version 1).xlsb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbval\Desktop\3Vikna\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomas\Desktop\3 vikna\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616D043E-1D8A-4BAC-B63A-E6D6B9665C36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E524AAE-87F6-4CDA-82F7-A662FF4F21B6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{292ADBA8-52A5-47D6-97C7-E12D992943EB}"/>
+    <workbookView xWindow="-8655" yWindow="465" windowWidth="18000" windowHeight="9360" xr2:uid="{292ADBA8-52A5-47D6-97C7-E12D992943EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="46">
   <si>
     <t>Number</t>
   </si>
@@ -63,15 +63,6 @@
     <t>Working catalogue site that lists all available products</t>
   </si>
   <si>
-    <t>Show name of product when clicking on it from the catalogue site</t>
-  </si>
-  <si>
-    <t>Show image of product when clicking on it from the catalogue site</t>
-  </si>
-  <si>
-    <t>Show description of product when clicking on it from the catalogue site</t>
-  </si>
-  <si>
     <t>Should be possible to filter by type of product on catalogue site</t>
   </si>
   <si>
@@ -175,6 +166,9 @@
   </si>
   <si>
     <t>Should be possible to remove a product from the cart</t>
+  </si>
+  <si>
+    <t>Show details of a product when clicking on it from the catalogue site</t>
   </si>
 </sst>
 </file>
@@ -557,22 +551,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A29ECF-1B85-49A7-9822-BF06B096B68E}">
-  <dimension ref="B3:F41"/>
+  <dimension ref="B3:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="72.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.265625" customWidth="1"/>
-    <col min="5" max="5" width="12.73046875" customWidth="1"/>
-    <col min="11" max="11" width="60.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="60.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -586,7 +580,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -594,35 +588,35 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>3</v>
       </c>
@@ -630,271 +624,271 @@
         <v>9</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>4</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>5</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>6</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>7</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>8</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <v>9</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>10</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
         <v>11</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
         <v>12</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
         <v>13</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
         <v>14</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
         <v>15</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B20" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20">
         <v>16</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B21" s="5">
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21">
         <v>17</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D26" t="s">
         <v>35</v>
@@ -903,12 +897,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D27" t="s">
         <v>35</v>
@@ -917,193 +911,165 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>24</v>
       </c>
       <c r="C28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
         <v>26</v>
       </c>
-      <c r="D28" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B29">
-        <v>25</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="D32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="3">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
         <v>36</v>
       </c>
-      <c r="D29" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B30">
-        <v>26</v>
-      </c>
-      <c r="C30" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" t="s">
-        <v>35</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B31" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
-        <v>28</v>
-      </c>
-      <c r="D32" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B33">
-        <v>2</v>
-      </c>
-      <c r="C33" t="s">
-        <v>43</v>
-      </c>
-      <c r="D33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B34">
-        <v>3</v>
-      </c>
-      <c r="C34" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34" t="s">
-        <v>35</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B35">
-        <v>4</v>
-      </c>
-      <c r="C35" t="s">
-        <v>30</v>
-      </c>
-      <c r="D35" t="s">
-        <v>35</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B36">
-        <v>5</v>
-      </c>
-      <c r="C36" t="s">
-        <v>42</v>
-      </c>
-      <c r="D36" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B37">
-        <v>6</v>
-      </c>
-      <c r="C37" t="s">
-        <v>32</v>
-      </c>
-      <c r="D37" t="s">
-        <v>35</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B38">
-        <v>7</v>
-      </c>
-      <c r="C38" t="s">
-        <v>31</v>
-      </c>
       <c r="D38" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B40" s="3">
-        <v>9</v>
-      </c>
-      <c r="C40" t="s">
-        <v>39</v>
-      </c>
-      <c r="D40" t="s">
-        <v>34</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B41">
-        <v>10</v>
-      </c>
-      <c r="C41" t="s">
-        <v>40</v>
-      </c>
-      <c r="D41" t="s">
-        <v>34</v>
-      </c>
-      <c r="E41" s="4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
merged some like requirements
</commit_message>
<xml_diff>
--- a/requirements (version 1).xlsb.xlsx
+++ b/requirements (version 1).xlsb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomas\Desktop\3 vikna\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E524AAE-87F6-4CDA-82F7-A662FF4F21B6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCC8A45-1B34-47BA-898D-BB4AA2B431E3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8655" yWindow="465" windowWidth="18000" windowHeight="9360" xr2:uid="{292ADBA8-52A5-47D6-97C7-E12D992943EB}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="18000" windowHeight="9360" xr2:uid="{292ADBA8-52A5-47D6-97C7-E12D992943EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -551,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A29ECF-1B85-49A7-9822-BF06B096B68E}">
-  <dimension ref="B3:F39"/>
+  <dimension ref="B3:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,7 +975,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>4</v>
       </c>
@@ -989,7 +989,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>5</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>6</v>
       </c>
@@ -1016,8 +1016,12 @@
       <c r="E35" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>7</v>
       </c>
@@ -1030,8 +1034,12 @@
       <c r="E36" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>8</v>
       </c>
@@ -1044,8 +1052,12 @@
       <c r="E37" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="6"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="3">
         <v>9</v>
       </c>
@@ -1058,8 +1070,12 @@
       <c r="E38" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="6"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>10</v>
       </c>
@@ -1072,6 +1088,146 @@
       <c r="E39" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="6"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="6"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="6"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="6"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="6"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="6"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="6"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="6"/>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="6"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="6"/>
+    </row>
+    <row r="49" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="6"/>
+    </row>
+    <row r="50" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="6"/>
+    </row>
+    <row r="51" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="6"/>
+    </row>
+    <row r="52" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K52" s="4"/>
+    </row>
+    <row r="53" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K53" s="4"/>
+    </row>
+    <row r="54" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K54" s="4"/>
+    </row>
+    <row r="55" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K55" s="4"/>
+    </row>
+    <row r="56" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K56" s="4"/>
+    </row>
+    <row r="57" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K57" s="4"/>
+    </row>
+    <row r="58" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K58" s="4"/>
+    </row>
+    <row r="59" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K59" s="4"/>
+    </row>
+    <row r="60" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K60" s="4"/>
+    </row>
+    <row r="61" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+    </row>
+    <row r="62" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K62" s="4"/>
+    </row>
+    <row r="63" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K63" s="4"/>
+    </row>
+    <row r="64" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K64" s="4"/>
+    </row>
+    <row r="65" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K65" s="4"/>
+    </row>
+    <row r="66" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K66" s="4"/>
+    </row>
+    <row r="67" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K67" s="4"/>
+    </row>
+    <row r="68" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K68" s="4"/>
+    </row>
+    <row r="69" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K69" s="4"/>
+    </row>
+    <row r="70" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H70" s="3"/>
+      <c r="K70" s="4"/>
+    </row>
+    <row r="71" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K71" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>